<commit_message>
Added the updated version of c# from freddy to the project.
</commit_message>
<xml_diff>
--- a/Lab 5 SQL Example.xlsx
+++ b/Lab 5 SQL Example.xlsx
@@ -568,7 +568,7 @@
   <dimension ref="B3:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <f ca="1">NOW()</f>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -651,7 +651,7 @@
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <f t="shared" ref="B7:B25" ca="1" si="0">NOW()</f>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -675,7 +675,7 @@
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -699,7 +699,7 @@
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -723,7 +723,7 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -747,7 +747,7 @@
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -771,7 +771,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -795,7 +795,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -819,7 +819,7 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -843,7 +843,7 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -867,7 +867,7 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f ca="1">NOW()</f>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -891,7 +891,7 @@
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -915,7 +915,7 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -939,7 +939,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
@@ -963,7 +963,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -987,7 +987,7 @@
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
@@ -1011,7 +1011,7 @@
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
@@ -1035,7 +1035,7 @@
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -1059,7 +1059,7 @@
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
@@ -1083,7 +1083,7 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42407.842937384259</v>
+        <v>42409.743987731483</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>

</xml_diff>